<commit_message>
code clone without template effect
</commit_message>
<xml_diff>
--- a/ironhack/function_clone/dictionary/dictionary.xlsx
+++ b/ironhack/function_clone/dictionary/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles/Dropbox/graduation/thesis/function/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles/Programming/PythonPractice/ironhack/function_clone/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -312,7 +312,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +341,11 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="161"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -375,11 +380,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -891,7 +897,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D6" sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,205 +913,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1182,20 +1226,20 @@
         <v>74</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1213,23 +1257,23 @@
       <c r="E3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1248,23 +1292,23 @@
       <c r="E4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1283,23 +1327,23 @@
       <c r="E5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1318,23 +1362,23 @@
       <c r="E6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1399,7 +1443,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>